<commit_message>
Rework 1 stage v2
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Diplom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Diplom\Diploma-project-in-the-profession-of--Testing-Engineer-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA1B7A3-6B82-4917-A3B8-F4944F5EE120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE002045-07CC-4EDF-9176-AE87B4E771CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>№</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Функциональное тестирование</t>
   </si>
   <si>
-    <t>Работоспособность основного функционала приложения</t>
-  </si>
-  <si>
     <t>Сворачивание/разворачивание приложения</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Middle</t>
   </si>
   <si>
-    <t>Тестирование полей и виджетов</t>
-  </si>
-  <si>
     <t>Виджеты установки даты и времени</t>
   </si>
   <si>
@@ -163,6 +157,24 @@
   </si>
   <si>
     <t xml:space="preserve">Обязательные </t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>Не функциональное тестирование</t>
+  </si>
+  <si>
+    <t>Авторизация</t>
+  </si>
+  <si>
+    <t>Создание, удаление, редактирование и фильтрация новостей</t>
+  </si>
+  <si>
+    <t>Навигация в приложении</t>
+  </si>
+  <si>
+    <t>Тестирование полей</t>
   </si>
 </sst>
 </file>
@@ -344,7 +356,51 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -385,13 +441,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -451,14 +507,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -518,14 +574,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>241788</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -586,13 +642,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>200025</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>41764</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -719,14 +775,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>1</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -786,14 +842,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>14</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>1</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -853,14 +909,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>25</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>1</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -920,14 +976,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>241788</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -987,13 +1043,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1050,14 +1106,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>28</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41763"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>241788</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1110" name="Check Box 86" hidden="1">
@@ -1066,7 +1127,7 @@
                   <a14:compatExt spid="_x0000_s1110"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9F36129-294F-4DAD-87D6-232E55DDE371}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1106,6 +1167,269 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>41764</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1111" name="Check Box 87" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1111"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1112" name="Check Box 88" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1112"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1113" name="Check Box 89" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1113"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000059040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="47625"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1114" name="Check Box 90" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1114"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E6CCB9-DB48-438B-AEEE-2601AB58D4FE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
       </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
@@ -1116,19 +1440,453 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>30</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41763"/>
+        <xdr:ext cx="47625" cy="41764"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1111" name="Check Box 87" hidden="1">
+            <xdr:cNvPr id="1115" name="Check Box 91" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1111"/>
+                  <a14:compatExt spid="_x0000_s1115"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECE86AFE-F2DE-4B07-8277-6612764A3EB1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C769A4B-C98C-4589-8812-C88884C929EF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1116" name="Check Box 92" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1116"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8718EB2-A0B6-4E24-ACEA-29553478E60B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="47625"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1117" name="Check Box 93" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1117"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE76131F-F593-43C0-AF31-7C42CB00FE2C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1118" name="Check Box 94" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1118"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2671F589-3031-45EC-96B8-F064211DD8A8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1119" name="Check Box 95" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1119"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18EE5D23-B92B-4C2B-8E1C-8D450CBB2E4B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1120" name="Check Box 96" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1120"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E947647C-01C7-4B24-B202-93E74F95321E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="47625"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1121" name="Check Box 97" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1121"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52B70976-35E2-4CF0-87AA-E6422498A33D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1122" name="Check Box 98" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1122"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA0803F-D377-4314-8587-AD1564D2A0AF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1438,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1457,21 +2215,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="8"/>
@@ -1481,13 +2239,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1495,13 +2253,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,13 +2267,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>37</v>
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1523,9 +2281,9 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -1537,307 +2295,345 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>37</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="C11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
         <v>1</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>37</v>
+      <c r="C14" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>1</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
-        <v>5</v>
-      </c>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
+        <v>1</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="B23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
         <v>1</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="8"/>
+      <c r="C24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>1</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
-        <v>2</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="8"/>
+      <c r="D27" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="B29" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
+        <v>2</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
         <v>3</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>40</v>
+      <c r="B32" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1857,13 +2653,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1878,13 +2674,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>5</xdr:row>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>6</xdr:row>
+                    <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1900,13 +2696,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>4</xdr:row>
+                    <xdr:row>3</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>5</xdr:row>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1923,13 +2719,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>200025</xdr:rowOff>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1966,13 +2762,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>11</xdr:row>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>12</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1988,13 +2784,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>14</xdr:row>
+                    <xdr:row>13</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>15</xdr:row>
+                    <xdr:row>14</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2010,13 +2806,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>25</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2032,13 +2828,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>25</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>26</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2054,13 +2850,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2076,13 +2872,13 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>28</xdr:row>
+                    <xdr:row>27</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>29</xdr:row>
+                    <xdr:row>28</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2098,6 +2894,50 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1112" r:id="rId16" name="Check Box 88">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1113" r:id="rId17" name="Check Box 89">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>200025</xdr:rowOff>
                   </from>
@@ -2105,6 +2945,204 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>30</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1114" r:id="rId18" name="Check Box 90">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1115" r:id="rId19" name="Check Box 91">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1116" r:id="rId20" name="Check Box 92">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1117" r:id="rId21" name="Check Box 93">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1118" r:id="rId22" name="Check Box 94">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1119" r:id="rId23" name="Check Box 95">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1120" r:id="rId24" name="Check Box 96">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1121" r:id="rId25" name="Check Box 97">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>161925</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1122" r:id="rId26" name="Check Box 98">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>33</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>

<commit_message>
Added autotests and additional documentation.
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Diplom\Diploma-project-in-the-profession-of--Testing-Engineer-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE002045-07CC-4EDF-9176-AE87B4E771CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC686E3-2B50-4BB4-91E3-21C9450782A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>№</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>pass</t>
-  </si>
-  <si>
-    <t>fail</t>
   </si>
   <si>
     <t>8.</t>
@@ -181,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,13 +211,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF4A4A4A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -229,18 +219,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -288,39 +272,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -404,7 +386,55 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -514,7 +544,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -580,8 +610,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>241788</xdr:rowOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -648,7 +678,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>41764</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -782,7 +812,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -849,7 +879,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -916,7 +946,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -982,8 +1012,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>241788</xdr:rowOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1049,8 +1079,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>2801</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1116,8 +1146,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>241788</xdr:rowOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1184,7 +1214,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>41764</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1374,14 +1404,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="47625"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1114" name="Check Box 90" hidden="1">
@@ -1390,7 +1425,7 @@
                   <a14:compatExt spid="_x0000_s1114"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E6CCB9-DB48-438B-AEEE-2601AB58D4FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1430,20 +1465,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1115" name="Check Box 91" hidden="1">
@@ -1452,7 +1492,7 @@
                   <a14:compatExt spid="_x0000_s1115"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C769A4B-C98C-4589-8812-C88884C929EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1492,20 +1532,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1116" name="Check Box 92" hidden="1">
@@ -1514,7 +1559,7 @@
                   <a14:compatExt spid="_x0000_s1116"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8718EB2-A0B6-4E24-ACEA-29553478E60B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1554,20 +1599,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="47625"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1117" name="Check Box 93" hidden="1">
@@ -1576,7 +1626,7 @@
                   <a14:compatExt spid="_x0000_s1117"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE76131F-F593-43C0-AF31-7C42CB00FE2C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1616,20 +1666,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1118" name="Check Box 94" hidden="1">
@@ -1638,7 +1693,7 @@
                   <a14:compatExt spid="_x0000_s1118"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2671F589-3031-45EC-96B8-F064211DD8A8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1678,20 +1733,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1119" name="Check Box 95" hidden="1">
@@ -1700,7 +1760,7 @@
                   <a14:compatExt spid="_x0000_s1119"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18EE5D23-B92B-4C2B-8E1C-8D450CBB2E4B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1740,20 +1800,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1120" name="Check Box 96" hidden="1">
@@ -1762,7 +1827,7 @@
                   <a14:compatExt spid="_x0000_s1120"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E947647C-01C7-4B24-B202-93E74F95321E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1802,20 +1867,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="47625"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1121" name="Check Box 97" hidden="1">
@@ -1824,7 +1894,7 @@
                   <a14:compatExt spid="_x0000_s1121"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52B70976-35E2-4CF0-87AA-E6422498A33D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1864,6 +1934,135 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1122" name="Check Box 98" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1122"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1123" name="Check Box 99" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1123"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79F88E6B-E1A8-469F-A5BA-9CECA2E4AE98}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
       </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
@@ -1874,19 +2073,639 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>200025</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="47625" cy="41764"/>
+        <xdr:ext cx="47625" cy="35299"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1122" name="Check Box 98" hidden="1">
+            <xdr:cNvPr id="1124" name="Check Box 100" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1122"/>
+                  <a14:compatExt spid="_x0000_s1124"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA0803F-D377-4314-8587-AD1564D2A0AF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0059C296-5FB7-46E2-B24F-F907A7F87CDB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1125" name="Check Box 101" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1125"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE5874A9-6AEA-4FB3-8465-9D27C0FAE051}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1126" name="Check Box 102" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1126"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB4DA9AE-61C9-4FF5-AD2B-D12504F0976C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1127" name="Check Box 103" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1127"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C47B72-EFAF-4734-9640-C543FDF2D749}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1128" name="Check Box 104" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1128"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B77B841D-404A-461F-9E93-A531164DC472}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1129" name="Check Box 105" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1129"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1A6AAA-1F92-4E35-B974-ACAC689CF5DE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1130" name="Check Box 106" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1130"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89FB2143-966C-495B-8494-12A741E38C04}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1131" name="Check Box 107" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1131"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7AC54FA-9536-43DF-B413-1E5D031EB948}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1132" name="Check Box 108" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1132"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B9CE80F-3821-4971-BD08-F8EBCB37BA4E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1133" name="Check Box 109" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1133"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF1DECA4-1B31-48E2-B9AE-79B12EA4FB8C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="47625" cy="35299"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1134" name="Check Box 110" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1134"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B148719-F1D2-4432-BA2D-C675F090D072}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2199,441 +3018,441 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="113.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="113.42578125" style="9" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>45</v>
+      <c r="B2" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="8"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>38</v>
+      <c r="D3" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>40</v>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>38</v>
+      <c r="D5" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>39</v>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="8"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>40</v>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>39</v>
+      <c r="D11" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="8"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>40</v>
+      <c r="C13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>40</v>
+      <c r="D14" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>38</v>
+      <c r="C16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>2</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>38</v>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="7">
         <v>3</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>40</v>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>38</v>
+      <c r="C19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>39</v>
+      <c r="C20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="A22" s="7">
         <v>1</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>40</v>
+      <c r="D22" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="8"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>40</v>
+      <c r="D24" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+      <c r="A25" s="7">
         <v>2</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>40</v>
+      <c r="D25" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>49</v>
+      <c r="A26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>1</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>39</v>
+      <c r="B27" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="A28" s="7">
         <v>2</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>39</v>
+      <c r="B28" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="13" t="s">
+      <c r="A29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="8"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+      <c r="A30" s="7">
         <v>1</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>38</v>
+      <c r="D30" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="A31" s="7">
         <v>2</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>38</v>
+      <c r="D31" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
+      <c r="A32" s="7">
         <v>3</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>38</v>
+      <c r="D32" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="A33" s="7">
         <v>4</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>38</v>
+      <c r="D33" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3150,6 +3969,270 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1123" r:id="rId27" name="Check Box 99">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1124" r:id="rId28" name="Check Box 100">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1125" r:id="rId29" name="Check Box 101">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1126" r:id="rId30" name="Check Box 102">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1127" r:id="rId31" name="Check Box 103">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1128" r:id="rId32" name="Check Box 104">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1129" r:id="rId33" name="Check Box 105">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1130" r:id="rId34" name="Check Box 106">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1131" r:id="rId35" name="Check Box 107">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1132" r:id="rId36" name="Check Box 108">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1133" r:id="rId37" name="Check Box 109">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1134" r:id="rId38" name="Check Box 110">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>200025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>28</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>